<commit_message>
paper draft v3 graphs and analysis
</commit_message>
<xml_diff>
--- a/Figure Generating/taxon_transposases_summary.xlsx
+++ b/Figure Generating/taxon_transposases_summary.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin Juntao\Desktop\transposase-deep-ocean\Figure Generating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D96856C-A246-464B-89FA-6660016B065E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C0BE8A-125C-4BBD-A018-B87FEDA8EC0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12492" yWindow="1080" windowWidth="10644" windowHeight="9660" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="taxon_transposases_summary" sheetId="1" r:id="rId1"/>
     <sheet name="backup2" sheetId="3" r:id="rId2"/>
-    <sheet name="backup" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="backup" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="56">
   <si>
     <t>DCM</t>
   </si>
@@ -169,12 +171,92 @@
   <si>
     <t>Average ORF count per MAG</t>
   </si>
+  <si>
+    <t>Deep Malaspina</t>
+  </si>
+  <si>
+    <t>Transposase Abundance</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Bacteroidia</t>
+  </si>
+  <si>
+    <t>Dehalococcoidia</t>
+  </si>
+  <si>
+    <t>Others Or Unknown</t>
+  </si>
+  <si>
+    <t>Verrucomicrobia</t>
+  </si>
+  <si>
+    <t>Taxonomic Class with ≥ 10 MAGs</t>
+  </si>
+  <si>
+    <t>* Marinisomatia</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>average (inlcude all other taxonomical classes)</t>
+  </si>
+  <si>
+    <t>high-transposase (Alpha-, Beta-, Gammaproteobacteria, and Actinobacteria)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MAG category (group by </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>low-transposase (Flavobacteria, Acidimicrobidae, Gemmatimonadetes, Marinisomatia, and SAR202-2)</t>
+  </si>
+  <si>
+    <t>SRF &amp; DCM (shallow waters)</t>
+  </si>
+  <si>
+    <t>MES &amp; BAT (deep waters)</t>
+  </si>
+  <si>
+    <t>% of MAGs in deep waters</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,8 +397,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,6 +590,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -823,7 +925,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -875,6 +977,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3400,10 +3511,402 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA5A7BF-6E9C-4459-86A7-165CAE116E6F}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>43</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>72</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>122</v>
+      </c>
+      <c r="E8">
+        <v>67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+      <c r="C10">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>140</v>
+      </c>
+      <c r="E10">
+        <v>82</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>72</v>
+      </c>
+      <c r="C16">
+        <v>94</v>
+      </c>
+      <c r="D16">
+        <v>66</v>
+      </c>
+      <c r="E16">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F21">
+    <sortCondition ref="F2:F21"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A4AD09-1301-40D3-8FE2-8ECEA5777650}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -4217,4 +4720,112 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1512BBF2-B5D1-42A4-8DC8-6D161DA1D806}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1">
+        <v>241</v>
+      </c>
+      <c r="C2" s="1">
+        <v>416</v>
+      </c>
+      <c r="D2" s="20">
+        <f>C2/E2*100</f>
+        <v>63.318112633181123</v>
+      </c>
+      <c r="E2" s="1">
+        <f>B2+C2</f>
+        <v>657</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1">
+        <v>177</v>
+      </c>
+      <c r="C3" s="1">
+        <v>108</v>
+      </c>
+      <c r="D3" s="20">
+        <f t="shared" ref="D3" si="0">C3/E3*100</f>
+        <v>37.894736842105267</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3" si="1">B3+C3</f>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1">
+        <v>267</v>
+      </c>
+      <c r="C4" s="1">
+        <v>218</v>
+      </c>
+      <c r="D4" s="20">
+        <f>C4/E4*100</f>
+        <v>44.948453608247426</v>
+      </c>
+      <c r="E4" s="1">
+        <f>B4+C4</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>